<commit_message>
graficar en excel subido en carpeta deberes
antes solo estaba en el archivo Z1 en la carpeta de pandas
</commit_message>
<xml_diff>
--- a/Pandas/data/chart.xlsx
+++ b/Pandas/data/chart.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="JAJA" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -99,16 +99,43 @@
             <c:symbol val="circle"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$3:$A$6</c:f>
-            </c:numRef>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Ipsum</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dolor</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sit</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Amet</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$3:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="0"/>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -159,16 +186,43 @@
             <c:symbol val="circle"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$3:$A$6</c:f>
-            </c:numRef>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Ipsum</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dolor</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sit</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Amet</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$3:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="0"/>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -182,7 +236,6 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50020002"/>
         <c:crosses val="autoZero"/>

</xml_diff>